<commit_message>
bug removal listing wrong answers, new imgs for IE, JQuery for Remove method
</commit_message>
<xml_diff>
--- a/woorden.xlsx
+++ b/woorden.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="459">
   <si>
     <t>is</t>
   </si>
@@ -1371,6 +1371,33 @@
   </si>
   <si>
     <t>https://pixabay.com/nl/meisje-jurk-edelstaal-bloem-306525/</t>
+  </si>
+  <si>
+    <t>https://pixabay.com/nl/comic-stripfiguren-deadpan-emotie-2026759/</t>
+  </si>
+  <si>
+    <t>undefined.png</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>wrong.png</t>
+  </si>
+  <si>
+    <t>correct.png</t>
+  </si>
+  <si>
+    <t>https://pixabay.com/nl/smiley-groene-eenvoudige-gelukkig-146093/</t>
+  </si>
+  <si>
+    <t>https://pixabay.com/nl/smiley-groene-eenvoudige-ongelukkig-146094/</t>
   </si>
 </sst>
 </file>
@@ -1755,16 +1782,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1778,7 +1805,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1786,7 +1813,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1797,7 +1824,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +1832,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1816,7 +1843,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1827,7 +1854,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -1838,7 +1865,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>128</v>
       </c>
@@ -1849,7 +1876,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1860,7 +1887,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="10" spans="1:3" hidden="1">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1871,7 +1898,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1882,7 +1909,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>127</v>
       </c>
@@ -1893,7 +1920,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:3" hidden="1">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1901,7 +1928,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1912,7 +1939,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1923,7 +1950,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -1934,7 +1961,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="17" spans="1:3" hidden="1">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>113</v>
       </c>
@@ -1945,7 +1972,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="18" spans="1:3" hidden="1">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>120</v>
       </c>
@@ -1956,7 +1983,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>105</v>
       </c>
@@ -1967,7 +1994,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1978,7 +2005,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="21" spans="1:3" hidden="1">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -1989,7 +2016,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2000,7 +2027,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>68</v>
       </c>
@@ -2011,7 +2038,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -2022,7 +2049,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2033,7 +2060,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2044,7 +2071,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -2055,7 +2082,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -2063,7 +2090,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>91</v>
       </c>
@@ -2074,7 +2101,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="30" spans="1:3" hidden="1">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>137</v>
       </c>
@@ -2085,7 +2112,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="1:3" hidden="1">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -2096,7 +2123,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="32" spans="1:3" hidden="1">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2104,7 +2131,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>115</v>
       </c>
@@ -2112,7 +2139,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -2123,7 +2150,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>107</v>
       </c>
@@ -2131,7 +2158,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:3" hidden="1">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>108</v>
       </c>
@@ -2139,7 +2166,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -2147,7 +2174,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -2155,7 +2182,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2166,7 +2193,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -2177,7 +2204,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2188,7 +2215,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -2199,7 +2226,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -2210,7 +2237,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -2218,7 +2245,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:3" hidden="1">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2226,7 +2253,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:3" hidden="1">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>139</v>
       </c>
@@ -2237,7 +2264,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="47" spans="1:3" hidden="1">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>168</v>
       </c>
@@ -2248,7 +2275,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="48" spans="1:3" hidden="1">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>130</v>
       </c>
@@ -2256,7 +2283,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>135</v>
       </c>
@@ -2267,7 +2294,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="50" spans="1:3" hidden="1">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>150</v>
       </c>
@@ -2278,7 +2305,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>149</v>
       </c>
@@ -2289,7 +2316,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>121</v>
       </c>
@@ -2300,7 +2327,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="53" spans="1:3" hidden="1">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>124</v>
       </c>
@@ -2311,7 +2338,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="54" spans="1:3" hidden="1">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>151</v>
       </c>
@@ -2322,7 +2349,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="55" spans="1:3" hidden="1">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>138</v>
       </c>
@@ -2333,7 +2360,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="56" spans="1:3" hidden="1">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>148</v>
       </c>
@@ -2344,7 +2371,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="57" spans="1:3" hidden="1">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>123</v>
       </c>
@@ -2352,7 +2379,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:3" hidden="1">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>81</v>
       </c>
@@ -2363,7 +2390,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="1:3" hidden="1">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>5</v>
       </c>
@@ -2371,7 +2398,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="60" spans="1:3" hidden="1">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -2379,7 +2406,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:3" hidden="1">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>27</v>
       </c>
@@ -2387,7 +2414,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:3" hidden="1">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -2395,7 +2422,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:3" hidden="1">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -2406,7 +2433,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>28</v>
       </c>
@@ -2417,7 +2444,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -2428,7 +2455,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2436,7 +2463,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>14</v>
       </c>
@@ -2447,7 +2474,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -2458,7 +2485,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -2466,7 +2493,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>132</v>
       </c>
@@ -2474,7 +2501,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>143</v>
       </c>
@@ -2482,7 +2509,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -2493,7 +2520,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -2504,7 +2531,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>109</v>
       </c>
@@ -2515,7 +2542,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>126</v>
       </c>
@@ -2523,7 +2550,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>110</v>
       </c>
@@ -2534,7 +2561,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>106</v>
       </c>
@@ -2545,7 +2572,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>96</v>
       </c>
@@ -2553,7 +2580,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -2561,7 +2588,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>44</v>
       </c>
@@ -2569,7 +2596,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>47</v>
       </c>
@@ -2577,7 +2604,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>46</v>
       </c>
@@ -2588,7 +2615,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -2596,7 +2623,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="84" spans="1:3" hidden="1">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>54</v>
       </c>
@@ -2607,7 +2634,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="85" spans="1:3" hidden="1">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>62</v>
       </c>
@@ -2618,7 +2645,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="86" spans="1:3" hidden="1">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>69</v>
       </c>
@@ -2626,7 +2653,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:3" hidden="1">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>64</v>
       </c>
@@ -2637,7 +2664,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="88" spans="1:3" hidden="1">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -2648,7 +2675,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="89" spans="1:3" hidden="1">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2659,7 +2686,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="90" spans="1:3" hidden="1">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -2670,7 +2697,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="91" spans="1:3" hidden="1">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -2681,7 +2708,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="92" spans="1:3" hidden="1">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -2692,7 +2719,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="93" spans="1:3" hidden="1">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>134</v>
       </c>
@@ -2703,7 +2730,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="94" spans="1:3" hidden="1">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>146</v>
       </c>
@@ -2714,7 +2741,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="95" spans="1:3" hidden="1">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>67</v>
       </c>
@@ -2725,7 +2752,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="96" spans="1:3" hidden="1">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>84</v>
       </c>
@@ -2736,7 +2763,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="97" spans="1:3" hidden="1">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>21</v>
       </c>
@@ -2747,7 +2774,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>114</v>
       </c>
@@ -2758,7 +2785,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="99" spans="1:3" hidden="1">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>72</v>
       </c>
@@ -2766,7 +2793,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="100" spans="1:3" hidden="1">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>63</v>
       </c>
@@ -2777,7 +2804,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>142</v>
       </c>
@@ -2788,7 +2815,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="102" spans="1:3" hidden="1">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -2799,7 +2826,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="103" spans="1:3" hidden="1">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -2810,7 +2837,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="104" spans="1:3" hidden="1">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -2821,7 +2848,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="105" spans="1:3" hidden="1">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>31</v>
       </c>
@@ -2832,7 +2859,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="106" spans="1:3" hidden="1">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>32</v>
       </c>
@@ -2843,7 +2870,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="107" spans="1:3" hidden="1">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>129</v>
       </c>
@@ -2854,7 +2881,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="108" spans="1:3" hidden="1">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>15</v>
       </c>
@@ -2865,7 +2892,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="109" spans="1:3" hidden="1">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>87</v>
       </c>
@@ -2876,7 +2903,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="110" spans="1:3" hidden="1">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>131</v>
       </c>
@@ -2887,7 +2914,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="111" spans="1:3" hidden="1">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>136</v>
       </c>
@@ -2898,7 +2925,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="112" spans="1:3" hidden="1">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>144</v>
       </c>
@@ -2909,7 +2936,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="113" spans="1:3" hidden="1">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>145</v>
       </c>
@@ -2917,7 +2944,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="114" spans="1:3" hidden="1">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -2928,7 +2955,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>93</v>
       </c>
@@ -2939,7 +2966,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>101</v>
       </c>
@@ -2947,7 +2974,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="117" spans="1:3" hidden="1">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>102</v>
       </c>
@@ -2958,7 +2985,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="118" spans="1:3" hidden="1">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>103</v>
       </c>
@@ -2969,7 +2996,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="119" spans="1:3" hidden="1">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>98</v>
       </c>
@@ -2980,7 +3007,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:3" hidden="1">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>122</v>
       </c>
@@ -2991,7 +3018,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="121" spans="1:3" hidden="1">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>58</v>
       </c>
@@ -3002,7 +3029,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="122" spans="1:3" hidden="1">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>57</v>
       </c>
@@ -3013,7 +3040,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="123" spans="1:3" hidden="1">
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -3024,7 +3051,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="124" spans="1:3" hidden="1">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -3035,7 +3062,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="125" spans="1:3" hidden="1">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -3046,7 +3073,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="126" spans="1:3" hidden="1">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>147</v>
       </c>
@@ -3057,7 +3084,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="127" spans="1:3" hidden="1">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>42</v>
       </c>
@@ -3068,7 +3095,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="128" spans="1:3" hidden="1">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>119</v>
       </c>
@@ -3079,7 +3106,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="129" spans="1:3" hidden="1">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>82</v>
       </c>
@@ -3090,7 +3117,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="130" spans="1:3" hidden="1">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>85</v>
       </c>
@@ -3101,7 +3128,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="131" spans="1:3" hidden="1">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -3112,7 +3139,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:3" hidden="1">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>112</v>
       </c>
@@ -3123,7 +3150,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>71</v>
       </c>
@@ -3131,7 +3158,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="134" spans="1:3" hidden="1">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>4</v>
       </c>
@@ -3142,7 +3169,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="135" spans="1:3" hidden="1">
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
         <v>8</v>
       </c>
@@ -3153,7 +3180,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="136" spans="1:3" hidden="1">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>22</v>
       </c>
@@ -3164,7 +3191,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="137" spans="1:3" hidden="1">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>83</v>
       </c>
@@ -3175,7 +3202,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="138" spans="1:3" hidden="1">
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>30</v>
       </c>
@@ -3186,7 +3213,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="139" spans="1:3" hidden="1">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>40</v>
       </c>
@@ -3197,7 +3224,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="140" spans="1:3" hidden="1">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>12</v>
       </c>
@@ -3219,7 +3246,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="142" spans="1:3" hidden="1">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>34</v>
       </c>
@@ -3230,7 +3257,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="143" spans="1:3" hidden="1">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -3241,7 +3268,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="144" spans="1:3" hidden="1">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>111</v>
       </c>
@@ -3252,7 +3279,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="145" spans="1:3" hidden="1">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>99</v>
       </c>
@@ -3263,7 +3290,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="146" spans="1:3" hidden="1">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>66</v>
       </c>
@@ -3274,7 +3301,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="147" spans="1:3" hidden="1">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>162</v>
       </c>
@@ -3282,7 +3309,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="148" spans="1:3" hidden="1">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>157</v>
       </c>
@@ -3293,7 +3320,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="149" spans="1:3" hidden="1">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>160</v>
       </c>
@@ -3301,7 +3328,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>158</v>
       </c>
@@ -3312,7 +3339,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="151" spans="1:3" hidden="1">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>159</v>
       </c>
@@ -3320,7 +3347,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="152" spans="1:3" hidden="1">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -3331,7 +3358,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="153" spans="1:3" hidden="1">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -3342,7 +3369,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="154" spans="1:3" hidden="1">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>165</v>
       </c>
@@ -3353,7 +3380,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="155" spans="1:3" hidden="1">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -3361,7 +3388,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="156" spans="1:3" hidden="1">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>167</v>
       </c>
@@ -3372,7 +3399,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="157" spans="1:3" hidden="1">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>161</v>
       </c>
@@ -3383,7 +3410,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="158" spans="1:3" hidden="1">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>153</v>
       </c>
@@ -3394,7 +3421,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="159" spans="1:3" hidden="1">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -3405,7 +3432,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>155</v>
       </c>
@@ -3416,7 +3443,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="161" spans="1:3" hidden="1">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>154</v>
       </c>
@@ -3427,7 +3454,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="162" spans="1:3" hidden="1">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -3438,13 +3465,45 @@
         <v>439</v>
       </c>
     </row>
+    <row r="163" spans="1:3">
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>452</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="C164" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>453</v>
+      </c>
+      <c r="B165" t="s">
+        <v>455</v>
+      </c>
+      <c r="C165" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>454</v>
+      </c>
+      <c r="B166" t="s">
+        <v>456</v>
+      </c>
+      <c r="C166" t="s">
+        <v>457</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C162">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="vet"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="0"/>
     <filterColumn colId="2"/>
   </autoFilter>
   <sortState ref="A1:A162">

</xml_diff>